<commit_message>
refactor: Complete folder restructuring for mooring-tension-iteration tests
- Eliminated hidden dot-prefixed folders for cross-platform compatibility
- Restructured directories: .dat/ → run_files/dat/, .sim/ → run_files/sim/, .csv/ → collate/csv/
- Updated all YAML configs with new relative paths (../../ prefix)
- Fixed all shell scripts (dm_iterator.sh, dm_pretension_iteration.sh) with new paths
- Moved config files to organized scripts/config/ subdirectory
- Created helper scripts (run_test.py, run_test.sh) for testing
- Added visualization settings to sb configuration
- Generated complete visualization set for both pb and sb configurations
- Documented all path changes in PATH_UPDATES.md
- Successfully tested full pipeline with 20 CSV outputs and 8 visualizations
</commit_message>
<xml_diff>
--- a/tests/modules/orcaflex/mooring-tension-iteration/fsts-l015-test-cases/output/collate/pretension_analysis_summary.xlsx
+++ b/tests/modules/orcaflex/mooring-tension-iteration/fsts-l015-test-cases/output/collate/pretension_analysis_summary.xlsx
@@ -1170,7 +1170,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>D:/github/digitalmodel/specs/modules/orcaflex/mooring-tension-iteration/go-by/.sim/fsts_l015_hwl_125km3_l100_pb_vessel_statics_6dof.sim</t>
+          <t>D:/github/digitalmodel/tests/modules/orcaflex/mooring-tension-iteration/fsts-l015-test-cases/run_files/sim/fsts_l015_hwl_125km3_l100_pb_vessel_statics_6dof.sim</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1243,7 +1243,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D:/github/digitalmodel/specs/modules/orcaflex/mooring-tension-iteration/go-by/.sim/fsts_l015_hwl_125km3_l100_sb_vessel_statics_6dof.sim</t>
+          <t>D:/github/digitalmodel/tests/modules/orcaflex/mooring-tension-iteration/fsts-l015-test-cases/run_files/sim/fsts_l015_hwl_125km3_l100_sb_vessel_statics_6dof.sim</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1413,7 +1413,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>D:/github/digitalmodel/specs/modules/orcaflex/mooring-tension-iteration/go-by/.sim/fsts_l015_hwl_125km3_l100_pb_vessel_statics_6dof.sim</t>
+          <t>D:/github/digitalmodel/tests/modules/orcaflex/mooring-tension-iteration/fsts-l015-test-cases/run_files/sim/fsts_l015_hwl_125km3_l100_pb_vessel_statics_6dof.sim</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1459,7 +1459,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D:/github/digitalmodel/specs/modules/orcaflex/mooring-tension-iteration/go-by/.sim/fsts_l015_hwl_125km3_l100_sb_vessel_statics_6dof.sim</t>
+          <t>D:/github/digitalmodel/tests/modules/orcaflex/mooring-tension-iteration/fsts-l015-test-cases/run_files/sim/fsts_l015_hwl_125km3_l100_sb_vessel_statics_6dof.sim</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1592,7 +1592,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>D:/github/digitalmodel/specs/modules/orcaflex/mooring-tension-iteration/go-by/.sim/fsts_l015_hwl_125km3_l100_pb_vessel_statics_6dof.sim</t>
+          <t>D:/github/digitalmodel/tests/modules/orcaflex/mooring-tension-iteration/fsts-l015-test-cases/run_files/sim/fsts_l015_hwl_125km3_l100_pb_vessel_statics_6dof.sim</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1637,7 +1637,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D:/github/digitalmodel/specs/modules/orcaflex/mooring-tension-iteration/go-by/.sim/fsts_l015_hwl_125km3_l100_sb_vessel_statics_6dof.sim</t>
+          <t>D:/github/digitalmodel/tests/modules/orcaflex/mooring-tension-iteration/fsts-l015-test-cases/run_files/sim/fsts_l015_hwl_125km3_l100_sb_vessel_statics_6dof.sim</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>